<commit_message>
Adding in functionality to generate organic and paid messages
</commit_message>
<xml_diff>
--- a/scripts/facebook_text_templates.xlsx
+++ b/scripts/facebook_text_templates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
   <si>
     <t>#</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Join researcher Principal Investigator’s Name at Keck Medicine of USC in fighting #disease. Please share this clinical trial http://bit.ly/1234567 with your network. Thank you!</t>
-  </si>
-  <si>
-    <t>Message Category: General, recruiting - User-friendly</t>
   </si>
   <si>
     <t>If you have been diagnosed with #disease, you may qualify for this important clinical trial at Keck Medicine of USC. See if you are eligible here: http://bit.ly/1234567.</t>
@@ -217,7 +214,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,14 +226,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF990000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,7 +254,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -288,66 +277,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -652,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,38 +947,42 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>3</v>
@@ -1046,7 +993,7 @@
     </row>
     <row r="36" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>3</v>
@@ -1057,7 +1004,7 @@
     </row>
     <row r="37" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>3</v>
@@ -1068,7 +1015,7 @@
     </row>
     <row r="38" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>3</v>
@@ -1077,9 +1024,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>3</v>
@@ -1088,9 +1035,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>3</v>
@@ -1099,31 +1046,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>3</v>
@@ -1134,7 +1081,7 @@
     </row>
     <row r="44" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>3</v>
@@ -1143,9 +1090,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>3</v>
@@ -1154,9 +1101,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>3</v>
@@ -1167,7 +1114,7 @@
     </row>
     <row r="47" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>3</v>
@@ -1178,7 +1125,7 @@
     </row>
     <row r="48" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>3</v>
@@ -1189,7 +1136,7 @@
     </row>
     <row r="49" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>3</v>
@@ -1198,20 +1145,20 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>3</v>
@@ -1220,9 +1167,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>3</v>
@@ -1231,9 +1178,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>3</v>
@@ -1244,7 +1191,7 @@
     </row>
     <row r="54" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>3</v>
@@ -1253,9 +1200,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>3</v>
@@ -1264,9 +1211,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>3</v>
@@ -1275,20 +1222,20 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>3</v>
@@ -1299,7 +1246,7 @@
     </row>
     <row r="59" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>3</v>
@@ -1310,7 +1257,7 @@
     </row>
     <row r="60" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>3</v>
@@ -1319,9 +1266,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>3</v>
@@ -1330,21 +1277,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
-        <v>60</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A32:C32"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="http://bit.ly/1234567"/>
     <hyperlink ref="C4" r:id="rId2" display="http://bit.ly/1234567"/>
@@ -1368,15 +1301,15 @@
     <hyperlink ref="C29" r:id="rId20" display="http://bit.ly/1234567"/>
     <hyperlink ref="C30" r:id="rId21" display="http://bit.ly/1234567"/>
     <hyperlink ref="C31" r:id="rId22" display="http://bit.ly/1234567with"/>
-    <hyperlink ref="C34" r:id="rId23" display="http://bit.ly/1234567"/>
-    <hyperlink ref="C42" r:id="rId24" display="http://bit.ly/1234567"/>
-    <hyperlink ref="C51" r:id="rId25" display="http://bit.ly/1234567"/>
-    <hyperlink ref="C52" r:id="rId26" display="http://bit.ly/1234567"/>
-    <hyperlink ref="C53" r:id="rId27" display="http://bit.ly/1234567"/>
-    <hyperlink ref="C54" r:id="rId28" display="http://bit.ly/1234567"/>
-    <hyperlink ref="C55" r:id="rId29" display="http://bit.ly/1234567"/>
-    <hyperlink ref="C56" r:id="rId30" display="http://bit.ly/1234567"/>
-    <hyperlink ref="C57" r:id="rId31" display="http://bit.ly/1234567"/>
+    <hyperlink ref="C33" r:id="rId23" display="http://bit.ly/1234567"/>
+    <hyperlink ref="C41" r:id="rId24" display="http://bit.ly/1234567"/>
+    <hyperlink ref="C50" r:id="rId25" display="http://bit.ly/1234567"/>
+    <hyperlink ref="C51" r:id="rId26" display="http://bit.ly/1234567"/>
+    <hyperlink ref="C52" r:id="rId27" display="http://bit.ly/1234567"/>
+    <hyperlink ref="C53" r:id="rId28" display="http://bit.ly/1234567"/>
+    <hyperlink ref="C54" r:id="rId29" display="http://bit.ly/1234567"/>
+    <hyperlink ref="C55" r:id="rId30" display="http://bit.ly/1234567"/>
+    <hyperlink ref="C56" r:id="rId31" display="http://bit.ly/1234567"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId32"/>

</xml_diff>